<commit_message>
minor tweaks on demo
</commit_message>
<xml_diff>
--- a/Tests/resources/test_actionpoint_config.xlsx
+++ b/Tests/resources/test_actionpoint_config.xlsx
@@ -8,93 +8,103 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git\HAL\HAL-Devices\Tests\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EFC4319-73FC-466A-825B-A81A43FE1C8E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37BBBD96-F972-40C2-A8D3-3B6BF58CFE1C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7980" tabRatio="791" activeTab="1" xr2:uid="{694A1011-F733-4B3D-865A-EAFA5EFA9CF7}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7980" tabRatio="791" activeTab="2" xr2:uid="{694A1011-F733-4B3D-865A-EAFA5EFA9CF7}"/>
   </bookViews>
   <sheets>
     <sheet name="Study" sheetId="3" r:id="rId1"/>
-    <sheet name="MainSupply.Temperature" sheetId="12" r:id="rId2"/>
-    <sheet name="MainSupply.Pressure" sheetId="13" r:id="rId3"/>
-    <sheet name="MainSupply.DewPoint" sheetId="11" r:id="rId4"/>
-    <sheet name="MainSupply.Humidity" sheetId="14" r:id="rId5"/>
-    <sheet name="MainSupply.H2OConcentration" sheetId="10" r:id="rId6"/>
-    <sheet name="Virtual NEO480 1" sheetId="8" r:id="rId7"/>
-    <sheet name="Virtual Thermometer" sheetId="9" r:id="rId8"/>
-    <sheet name="CAN1" sheetId="1" r:id="rId9"/>
-    <sheet name="PCAN_USBBUS1  0x51" sheetId="5" r:id="rId10"/>
-    <sheet name="cDAQ9191-TC" sheetId="6" r:id="rId11"/>
-    <sheet name="cDAQ9191-TC.ai0" sheetId="7" r:id="rId12"/>
+    <sheet name="Stack1.Temperature" sheetId="15" r:id="rId2"/>
+    <sheet name="Virtual Stack1.Temperature CSV" sheetId="16" r:id="rId3"/>
+    <sheet name="MainSupply.Temperature" sheetId="12" r:id="rId4"/>
+    <sheet name="MainSupply.Pressure" sheetId="13" r:id="rId5"/>
+    <sheet name="MainSupply.DewPoint" sheetId="11" r:id="rId6"/>
+    <sheet name="MainSupply.Humidity" sheetId="14" r:id="rId7"/>
+    <sheet name="MainSupply.H2OConcentration" sheetId="10" r:id="rId8"/>
+    <sheet name="Virtual NEO480 1" sheetId="8" r:id="rId9"/>
+    <sheet name="Virtual Thermometer" sheetId="9" r:id="rId10"/>
+    <sheet name="CAN1" sheetId="1" r:id="rId11"/>
+    <sheet name="PCAN_USBBUS1  0x51" sheetId="5" r:id="rId12"/>
+    <sheet name="cDAQ9191-TC" sheetId="6" r:id="rId13"/>
+    <sheet name="cDAQ9191-TC.ai0" sheetId="7" r:id="rId14"/>
   </sheets>
   <definedNames>
     <definedName name="ActionPoints" localSheetId="0">Study!$C$2:$C$21</definedName>
-    <definedName name="Attributes.Baudrate" localSheetId="8">'CAN1'!$B$5</definedName>
-    <definedName name="Attributes.Baudrate" localSheetId="9">'PCAN_USBBUS1  0x51'!$B$5</definedName>
-    <definedName name="Attributes.Channel" localSheetId="7">'Virtual Thermometer'!$B$5</definedName>
-    <definedName name="Attributes.Channels" localSheetId="10">'cDAQ9191-TC'!$B$6:$B$14</definedName>
-    <definedName name="Attributes.DataLogger.Class" localSheetId="3">MainSupply.DewPoint!$B$5</definedName>
-    <definedName name="Attributes.DataLogger.Class" localSheetId="5">MainSupply.H2OConcentration!$B$5</definedName>
-    <definedName name="Attributes.DataLogger.Class" localSheetId="4">MainSupply.Humidity!$B$5</definedName>
-    <definedName name="Attributes.DataLogger.Class" localSheetId="2">MainSupply.Pressure!$B$5</definedName>
-    <definedName name="Attributes.DataLogger.Class" localSheetId="1">MainSupply.Temperature!$B$5</definedName>
-    <definedName name="Attributes.DataLogger.Destination" localSheetId="3">MainSupply.DewPoint!$B$4</definedName>
-    <definedName name="Attributes.DataLogger.Destination" localSheetId="5">MainSupply.H2OConcentration!$B$4</definedName>
-    <definedName name="Attributes.DataLogger.Destination" localSheetId="4">MainSupply.Humidity!$B$4</definedName>
-    <definedName name="Attributes.DataLogger.Destination" localSheetId="2">MainSupply.Pressure!$B$4</definedName>
-    <definedName name="Attributes.DataLogger.Destination" localSheetId="1">MainSupply.Temperature!$B$4</definedName>
-    <definedName name="Attributes.DbcFilepath" localSheetId="8">'CAN1'!$B$7</definedName>
-    <definedName name="Attributes.DbcFilepath" localSheetId="9">'PCAN_USBBUS1  0x51'!$B$7</definedName>
-    <definedName name="Attributes.FrameName1" localSheetId="6">'Virtual NEO480 1'!$B$5</definedName>
-    <definedName name="Attributes.FrameName1" localSheetId="7">'Virtual Thermometer'!$B$5</definedName>
-    <definedName name="Attributes.FrameName2" localSheetId="6">'Virtual NEO480 1'!$B$6</definedName>
-    <definedName name="Attributes.FrameName2" localSheetId="7">'Virtual Thermometer'!$B$6</definedName>
-    <definedName name="Attributes.GrpcServerAddress" localSheetId="8">'CAN1'!$B$9</definedName>
-    <definedName name="Attributes.ReadRate" localSheetId="8">'CAN1'!$B$6</definedName>
-    <definedName name="Attributes.ReadRate" localSheetId="10">'cDAQ9191-TC'!$B$5</definedName>
-    <definedName name="Attributes.ReadRate" localSheetId="9">'PCAN_USBBUS1  0x51'!$B$6</definedName>
-    <definedName name="Attributes.Termination" localSheetId="8">'CAN1'!$B$8</definedName>
-    <definedName name="Attributes.Timing.ActiveEdge" localSheetId="10">'cDAQ9191-TC'!$B$21</definedName>
-    <definedName name="Attributes.Timing.SampleClockSource" localSheetId="10">'cDAQ9191-TC'!$B$20</definedName>
-    <definedName name="Attributes.Timing.SampleMode" localSheetId="10">'cDAQ9191-TC'!$B$18</definedName>
-    <definedName name="Attributes.Timing.SampleRate" localSheetId="10">'cDAQ9191-TC'!$B$19</definedName>
-    <definedName name="Attributes.Timing.SamplesPerChannel" localSheetId="10">'cDAQ9191-TC'!$B$17</definedName>
-    <definedName name="Attributes.Timing.Type" localSheetId="10">'cDAQ9191-TC'!$B$16</definedName>
-    <definedName name="Attributes.Trigger.TriggerType" localSheetId="10">'cDAQ9191-TC'!$B$23</definedName>
-    <definedName name="CjcChannel" localSheetId="11">'cDAQ9191-TC.ai0'!$B$7</definedName>
-    <definedName name="CjcSource" localSheetId="11">'cDAQ9191-TC.ai0'!$B$8</definedName>
-    <definedName name="CjcValue" localSheetId="11">'cDAQ9191-TC.ai0'!$B$9</definedName>
-    <definedName name="Class" localSheetId="8">'CAN1'!$B$2</definedName>
-    <definedName name="Class" localSheetId="10">'cDAQ9191-TC'!$B$2</definedName>
-    <definedName name="Class" localSheetId="9">'PCAN_USBBUS1  0x51'!$B$2</definedName>
-    <definedName name="Class" localSheetId="6">'Virtual NEO480 1'!$B$2</definedName>
-    <definedName name="Class" localSheetId="7">'Virtual Thermometer'!$B$2</definedName>
-    <definedName name="ConfigureClass" localSheetId="8">'CAN1'!$B$3</definedName>
-    <definedName name="ConfigureClass" localSheetId="10">'cDAQ9191-TC'!$B$3</definedName>
-    <definedName name="ConfigureClass" localSheetId="9">'PCAN_USBBUS1  0x51'!$B$3</definedName>
-    <definedName name="Enabled" localSheetId="11">'cDAQ9191-TC.ai0'!$B$2</definedName>
-    <definedName name="Identifier" localSheetId="3">MainSupply.DewPoint!$B$1</definedName>
-    <definedName name="Identifier" localSheetId="5">MainSupply.H2OConcentration!$B$1</definedName>
-    <definedName name="Identifier" localSheetId="4">MainSupply.Humidity!$B$1</definedName>
-    <definedName name="Identifier" localSheetId="2">MainSupply.Pressure!$B$1</definedName>
-    <definedName name="Identifier" localSheetId="1">MainSupply.Temperature!$B$1</definedName>
-    <definedName name="Identifier" localSheetId="6">'Virtual NEO480 1'!$B$1</definedName>
-    <definedName name="Identifier" localSheetId="7">'Virtual Thermometer'!$B$1</definedName>
-    <definedName name="Instrument" localSheetId="6">'Virtual NEO480 1'!$B$3</definedName>
-    <definedName name="Instrument" localSheetId="7">'Virtual Thermometer'!$B$3</definedName>
-    <definedName name="InstrumentIdentifier" localSheetId="8">'CAN1'!$B$1</definedName>
-    <definedName name="InstrumentIdentifier" localSheetId="10">'cDAQ9191-TC'!$B$1</definedName>
-    <definedName name="InstrumentIdentifier" localSheetId="9">'PCAN_USBBUS1  0x51'!$B$1</definedName>
+    <definedName name="Attributes.Alarming.Limits.Hi" localSheetId="1">Stack1.Temperature!$B$9</definedName>
+    <definedName name="Attributes.Alarming.Limits.HiHi" localSheetId="1">Stack1.Temperature!$B$8</definedName>
+    <definedName name="Attributes.Alarming.Limits.Lo" localSheetId="1">Stack1.Temperature!$B$10</definedName>
+    <definedName name="Attributes.Alarming.Limits.LoLo" localSheetId="1">Stack1.Temperature!$B$11</definedName>
+    <definedName name="Attributes.Baudrate" localSheetId="10">'CAN1'!$B$5</definedName>
+    <definedName name="Attributes.Baudrate" localSheetId="11">'PCAN_USBBUS1  0x51'!$B$5</definedName>
+    <definedName name="Attributes.Channel" localSheetId="9">'Virtual Thermometer'!$B$5</definedName>
+    <definedName name="Attributes.Channels" localSheetId="12">'cDAQ9191-TC'!$B$6:$B$14</definedName>
+    <definedName name="Attributes.DataLogger.Class" localSheetId="5">MainSupply.DewPoint!$B$5</definedName>
+    <definedName name="Attributes.DataLogger.Class" localSheetId="7">MainSupply.H2OConcentration!$B$5</definedName>
+    <definedName name="Attributes.DataLogger.Class" localSheetId="6">MainSupply.Humidity!$B$5</definedName>
+    <definedName name="Attributes.DataLogger.Class" localSheetId="4">MainSupply.Pressure!$B$5</definedName>
+    <definedName name="Attributes.DataLogger.Class" localSheetId="3">MainSupply.Temperature!$B$5</definedName>
+    <definedName name="Attributes.DataLogger.Class" localSheetId="1">Stack1.Temperature!$B$5</definedName>
+    <definedName name="Attributes.DataLogger.Destination" localSheetId="5">MainSupply.DewPoint!$B$4</definedName>
+    <definedName name="Attributes.DataLogger.Destination" localSheetId="7">MainSupply.H2OConcentration!$B$4</definedName>
+    <definedName name="Attributes.DataLogger.Destination" localSheetId="6">MainSupply.Humidity!$B$4</definedName>
+    <definedName name="Attributes.DataLogger.Destination" localSheetId="4">MainSupply.Pressure!$B$4</definedName>
+    <definedName name="Attributes.DataLogger.Destination" localSheetId="3">MainSupply.Temperature!$B$4</definedName>
+    <definedName name="Attributes.DataLogger.Destination" localSheetId="1">Stack1.Temperature!$B$4</definedName>
+    <definedName name="Attributes.DbcFilepath" localSheetId="10">'CAN1'!$B$7</definedName>
+    <definedName name="Attributes.DbcFilepath" localSheetId="11">'PCAN_USBBUS1  0x51'!$B$7</definedName>
+    <definedName name="Attributes.FrameName1" localSheetId="8">'Virtual NEO480 1'!$B$5</definedName>
+    <definedName name="Attributes.FrameName1" localSheetId="9">'Virtual Thermometer'!$B$5</definedName>
+    <definedName name="Attributes.FrameName2" localSheetId="8">'Virtual NEO480 1'!$B$6</definedName>
+    <definedName name="Attributes.FrameName2" localSheetId="9">'Virtual Thermometer'!$B$6</definedName>
+    <definedName name="Attributes.GrpcServerAddress" localSheetId="10">'CAN1'!$B$9</definedName>
+    <definedName name="Attributes.ReadRate" localSheetId="10">'CAN1'!$B$6</definedName>
+    <definedName name="Attributes.ReadRate" localSheetId="12">'cDAQ9191-TC'!$B$5</definedName>
+    <definedName name="Attributes.ReadRate" localSheetId="11">'PCAN_USBBUS1  0x51'!$B$6</definedName>
+    <definedName name="Attributes.Termination" localSheetId="10">'CAN1'!$B$8</definedName>
+    <definedName name="Attributes.Timing.ActiveEdge" localSheetId="12">'cDAQ9191-TC'!$B$21</definedName>
+    <definedName name="Attributes.Timing.SampleClockSource" localSheetId="12">'cDAQ9191-TC'!$B$20</definedName>
+    <definedName name="Attributes.Timing.SampleMode" localSheetId="12">'cDAQ9191-TC'!$B$18</definedName>
+    <definedName name="Attributes.Timing.SampleRate" localSheetId="12">'cDAQ9191-TC'!$B$19</definedName>
+    <definedName name="Attributes.Timing.SamplesPerChannel" localSheetId="12">'cDAQ9191-TC'!$B$17</definedName>
+    <definedName name="Attributes.Timing.Type" localSheetId="12">'cDAQ9191-TC'!$B$16</definedName>
+    <definedName name="Attributes.Trigger.TriggerType" localSheetId="12">'cDAQ9191-TC'!$B$23</definedName>
+    <definedName name="CjcChannel" localSheetId="13">'cDAQ9191-TC.ai0'!$B$7</definedName>
+    <definedName name="CjcSource" localSheetId="13">'cDAQ9191-TC.ai0'!$B$8</definedName>
+    <definedName name="CjcValue" localSheetId="13">'cDAQ9191-TC.ai0'!$B$9</definedName>
+    <definedName name="Class" localSheetId="10">'CAN1'!$B$2</definedName>
+    <definedName name="Class" localSheetId="12">'cDAQ9191-TC'!$B$2</definedName>
+    <definedName name="Class" localSheetId="11">'PCAN_USBBUS1  0x51'!$B$2</definedName>
+    <definedName name="Class" localSheetId="8">'Virtual NEO480 1'!$B$2</definedName>
+    <definedName name="Class" localSheetId="9">'Virtual Thermometer'!$B$2</definedName>
+    <definedName name="ConfigureClass" localSheetId="10">'CAN1'!$B$3</definedName>
+    <definedName name="ConfigureClass" localSheetId="12">'cDAQ9191-TC'!$B$3</definedName>
+    <definedName name="ConfigureClass" localSheetId="11">'PCAN_USBBUS1  0x51'!$B$3</definedName>
+    <definedName name="Enabled" localSheetId="13">'cDAQ9191-TC.ai0'!$B$2</definedName>
+    <definedName name="Identifier" localSheetId="5">MainSupply.DewPoint!$B$1</definedName>
+    <definedName name="Identifier" localSheetId="7">MainSupply.H2OConcentration!$B$1</definedName>
+    <definedName name="Identifier" localSheetId="6">MainSupply.Humidity!$B$1</definedName>
+    <definedName name="Identifier" localSheetId="4">MainSupply.Pressure!$B$1</definedName>
+    <definedName name="Identifier" localSheetId="3">MainSupply.Temperature!$B$1</definedName>
+    <definedName name="Identifier" localSheetId="1">Stack1.Temperature!$B$1</definedName>
+    <definedName name="Identifier" localSheetId="8">'Virtual NEO480 1'!$B$1</definedName>
+    <definedName name="Identifier" localSheetId="9">'Virtual Thermometer'!$B$1</definedName>
+    <definedName name="Instrument" localSheetId="8">'Virtual NEO480 1'!$B$3</definedName>
+    <definedName name="Instrument" localSheetId="9">'Virtual Thermometer'!$B$3</definedName>
+    <definedName name="InstrumentIdentifier" localSheetId="10">'CAN1'!$B$1</definedName>
+    <definedName name="InstrumentIdentifier" localSheetId="12">'cDAQ9191-TC'!$B$1</definedName>
+    <definedName name="InstrumentIdentifier" localSheetId="11">'PCAN_USBBUS1  0x51'!$B$1</definedName>
     <definedName name="Instruments" localSheetId="0">Study!$A$2:$A$21</definedName>
-    <definedName name="MaximumValue" localSheetId="11">'cDAQ9191-TC.ai0'!$B$4</definedName>
-    <definedName name="MinimumValue" localSheetId="11">'cDAQ9191-TC.ai0'!$B$3</definedName>
-    <definedName name="Name" localSheetId="11">'cDAQ9191-TC.ai0'!$B$1</definedName>
-    <definedName name="ThermocoupleType" localSheetId="11">'cDAQ9191-TC.ai0'!$B$5</definedName>
-    <definedName name="Units" localSheetId="11">'cDAQ9191-TC.ai0'!$B$6</definedName>
-    <definedName name="VirtualInstrument" localSheetId="3">MainSupply.DewPoint!$B$2</definedName>
-    <definedName name="VirtualInstrument" localSheetId="5">MainSupply.H2OConcentration!$B$2</definedName>
-    <definedName name="VirtualInstrument" localSheetId="4">MainSupply.Humidity!$B$2</definedName>
-    <definedName name="VirtualInstrument" localSheetId="2">MainSupply.Pressure!$B$2</definedName>
-    <definedName name="VirtualInstrument" localSheetId="1">MainSupply.Temperature!$B$2</definedName>
+    <definedName name="MaximumValue" localSheetId="13">'cDAQ9191-TC.ai0'!$B$4</definedName>
+    <definedName name="MinimumValue" localSheetId="13">'cDAQ9191-TC.ai0'!$B$3</definedName>
+    <definedName name="Name" localSheetId="13">'cDAQ9191-TC.ai0'!$B$1</definedName>
+    <definedName name="ThermocoupleType" localSheetId="13">'cDAQ9191-TC.ai0'!$B$5</definedName>
+    <definedName name="Units" localSheetId="13">'cDAQ9191-TC.ai0'!$B$6</definedName>
+    <definedName name="VirtualInstrument" localSheetId="5">MainSupply.DewPoint!$B$2</definedName>
+    <definedName name="VirtualInstrument" localSheetId="7">MainSupply.H2OConcentration!$B$2</definedName>
+    <definedName name="VirtualInstrument" localSheetId="6">MainSupply.Humidity!$B$2</definedName>
+    <definedName name="VirtualInstrument" localSheetId="4">MainSupply.Pressure!$B$2</definedName>
+    <definedName name="VirtualInstrument" localSheetId="3">MainSupply.Temperature!$B$2</definedName>
+    <definedName name="VirtualInstrument" localSheetId="1">Stack1.Temperature!$B$2</definedName>
     <definedName name="VirtualInstruments" localSheetId="0">Study!$B$2:$B$21</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -107,7 +117,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="123">
   <si>
     <t>InstrumentIdentifier</t>
   </si>
@@ -368,6 +378,114 @@
   </si>
   <si>
     <t>Attributes.Alarming.Limits.Lo-Lo</t>
+  </si>
+  <si>
+    <t>#Stack1.Temperature</t>
+  </si>
+  <si>
+    <t>#Stack2.Temperature</t>
+  </si>
+  <si>
+    <t>#Stack3.Temperature</t>
+  </si>
+  <si>
+    <t>#Stack4.Temperature</t>
+  </si>
+  <si>
+    <t>#Stack5.Temperature</t>
+  </si>
+  <si>
+    <t>#Stack6.Temperature</t>
+  </si>
+  <si>
+    <t>Stack1.Temperature</t>
+  </si>
+  <si>
+    <t>#Stack1.Fan</t>
+  </si>
+  <si>
+    <t>#Stack2.Fan</t>
+  </si>
+  <si>
+    <t>#Stack4.Fan</t>
+  </si>
+  <si>
+    <t>#Stack3.Fan</t>
+  </si>
+  <si>
+    <t>#Stack5.Fan</t>
+  </si>
+  <si>
+    <t>#Stack6.Fan</t>
+  </si>
+  <si>
+    <t>#Virtual Stack1.Temperature CSV</t>
+  </si>
+  <si>
+    <t>#Virtual Stack2.Temperature CSV</t>
+  </si>
+  <si>
+    <t>#Virtual Stack3.Temperature CSV</t>
+  </si>
+  <si>
+    <t>#Virtual Stack4.Temperature CSV</t>
+  </si>
+  <si>
+    <t>#Virtual Stack5.Temperature CSV</t>
+  </si>
+  <si>
+    <t>#Virtual Stack6.Temperature CSV</t>
+  </si>
+  <si>
+    <t>#Virtual Stack1.Fan CSV</t>
+  </si>
+  <si>
+    <t>#Virtual Stack2.Fan CSV</t>
+  </si>
+  <si>
+    <t>#Virtual Stack3.Fan CSV</t>
+  </si>
+  <si>
+    <t>#Virtual Stack4.Fan CSV</t>
+  </si>
+  <si>
+    <t>#Virtual Stack5.Fan CSV</t>
+  </si>
+  <si>
+    <t>#Virtual Stack6.Fan CSV</t>
+  </si>
+  <si>
+    <t>Virtual Stack1.Temperature CSV</t>
+  </si>
+  <si>
+    <t>Virtual Sensor from CSV.lvclass</t>
+  </si>
+  <si>
+    <t>Virtual Stack1.Thermometer CSV</t>
+  </si>
+  <si>
+    <t>Attributes.CsvParserClass</t>
+  </si>
+  <si>
+    <t>Attributes.CsvFilepath</t>
+  </si>
+  <si>
+    <t>Attributes.Input.Timestamp.Field</t>
+  </si>
+  <si>
+    <t>Time in sec</t>
+  </si>
+  <si>
+    <t>Attributes.Input.Timestamp.Format</t>
+  </si>
+  <si>
+    <t>Attributes.Input.Value.Field</t>
+  </si>
+  <si>
+    <t>%t</t>
+  </si>
+  <si>
+    <t>D:\\git\\HAL\\HAL-Devices\\Tests\\resources\\2024-11-27-17-48-50_Imponator_Last Hope.csv</t>
   </si>
 </sst>
 </file>
@@ -472,7 +590,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -488,7 +606,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -787,12 +905,13 @@
   <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="26.85546875" customWidth="1"/>
+    <col min="1" max="1" width="26.85546875" customWidth="1"/>
+    <col min="2" max="2" width="35.85546875" customWidth="1"/>
     <col min="3" max="3" width="29.42578125" customWidth="1"/>
     <col min="4" max="4" width="25.140625" customWidth="1"/>
   </cols>
@@ -834,84 +953,132 @@
       <c r="A4" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="B4" s="3"/>
+      <c r="B4" s="3" t="s">
+        <v>100</v>
+      </c>
       <c r="C4" s="6" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="3"/>
-      <c r="B5" s="3"/>
+      <c r="B5" s="3" t="s">
+        <v>101</v>
+      </c>
       <c r="C5" s="6" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="3"/>
-      <c r="B6" s="3"/>
+      <c r="B6" s="3" t="s">
+        <v>102</v>
+      </c>
       <c r="C6" s="6" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="3"/>
-      <c r="B7" s="3"/>
-      <c r="C7" s="6"/>
+      <c r="B7" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="3"/>
-      <c r="B8" s="3"/>
-      <c r="C8" s="6"/>
+      <c r="B8" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>88</v>
+      </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="3"/>
-      <c r="B9" s="3"/>
-      <c r="C9" s="6"/>
+      <c r="B9" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>89</v>
+      </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="3"/>
-      <c r="B10" s="3"/>
-      <c r="C10" s="6"/>
+      <c r="B10" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="3"/>
-      <c r="B11" s="3"/>
-      <c r="C11" s="6"/>
+      <c r="B11" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>91</v>
+      </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="3"/>
-      <c r="B12" s="3"/>
-      <c r="C12" s="6"/>
+      <c r="B12" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>92</v>
+      </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="3"/>
-      <c r="B13" s="3"/>
-      <c r="C13" s="6"/>
+      <c r="B13" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>94</v>
+      </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="3"/>
-      <c r="B14" s="3"/>
-      <c r="C14" s="6"/>
+      <c r="B14" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="3"/>
-      <c r="B15" s="3"/>
-      <c r="C15" s="6"/>
+      <c r="B15" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>97</v>
+      </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="3"/>
       <c r="B16" s="3"/>
-      <c r="C16" s="6"/>
+      <c r="C16" s="6" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="3"/>
       <c r="B17" s="3"/>
-      <c r="C17" s="6"/>
+      <c r="C17" s="6" t="s">
+        <v>98</v>
+      </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="3"/>
       <c r="B18" s="3"/>
-      <c r="C18" s="6"/>
+      <c r="C18" s="6" t="s">
+        <v>99</v>
+      </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="3"/>
@@ -934,6 +1101,141 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{700149C1-66F5-4A24-928F-5BBEDD6006E3}">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="25.5703125" customWidth="1"/>
+    <col min="2" max="2" width="29.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B3" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>79</v>
+      </c>
+      <c r="B5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A7DE5E1-2065-4857-A2CD-738C548B16E2}">
+  <dimension ref="A1:B9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="35.28515625" customWidth="1"/>
+    <col min="2" max="2" width="72" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>500000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>44</v>
+      </c>
+      <c r="B6">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6A9D403-72C5-472F-AC2B-4CAB762784A6}">
   <dimension ref="A1:B7"/>
   <sheetViews>
@@ -941,7 +1243,7 @@
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="36.140625" customWidth="1"/>
     <col min="2" max="2" width="72.42578125" customWidth="1"/>
@@ -1001,7 +1303,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1380816-54EF-4026-83D9-8EB7D75D6731}">
   <dimension ref="A1:B23"/>
   <sheetViews>
@@ -1009,7 +1311,7 @@
       <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="38.140625" customWidth="1"/>
     <col min="2" max="2" width="50.85546875" customWidth="1"/>
@@ -1117,7 +1419,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77D67891-1560-40D4-8A09-0C4C9BA29850}">
   <dimension ref="A1:B9"/>
   <sheetViews>
@@ -1125,7 +1427,7 @@
       <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.7109375" customWidth="1"/>
     <col min="2" max="2" width="16.5703125" customWidth="1"/>
@@ -1206,14 +1508,168 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5985D723-A6BE-40F0-A10F-877C7B68BD0A}">
+  <dimension ref="A1:B11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="31" customWidth="1"/>
+    <col min="2" max="2" width="30.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B2" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>83</v>
+      </c>
+      <c r="B8">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>84</v>
+      </c>
+      <c r="B9">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>85</v>
+      </c>
+      <c r="B10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>86</v>
+      </c>
+      <c r="B11">
+        <v>-1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44D00D5E-146F-4A24-B3DE-0097E54A6D7B}">
+  <dimension ref="A1:B9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="32.85546875" customWidth="1"/>
+    <col min="2" max="2" width="38.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>116</v>
+      </c>
+      <c r="B6" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>117</v>
+      </c>
+      <c r="B7" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>119</v>
+      </c>
+      <c r="B8" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>120</v>
+      </c>
+      <c r="B9" t="s">
+        <v>93</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F12D661-3DBC-4ACA-B17D-ECA2E2886AFC}">
   <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="34.85546875" customWidth="1"/>
     <col min="2" max="2" width="29.42578125" customWidth="1"/>
@@ -1276,7 +1732,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97B71A4A-0F0A-44DB-B525-8215CC86B044}">
   <dimension ref="A1:B9"/>
   <sheetViews>
@@ -1284,7 +1740,7 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="34.85546875" customWidth="1"/>
     <col min="2" max="2" width="29.42578125" customWidth="1"/>
@@ -1342,7 +1798,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09D25C40-8A50-421D-9AB2-EF8CA695243E}">
   <dimension ref="A1:B9"/>
   <sheetViews>
@@ -1350,7 +1806,7 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="34.85546875" customWidth="1"/>
     <col min="2" max="2" width="29.42578125" customWidth="1"/>
@@ -1408,7 +1864,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51A81152-973E-4DD3-BBA3-00065132513E}">
   <dimension ref="A1:B9"/>
   <sheetViews>
@@ -1416,7 +1872,7 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="34.85546875" customWidth="1"/>
     <col min="2" max="2" width="29.42578125" customWidth="1"/>
@@ -1474,7 +1930,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60A3EC77-AECF-4D53-8D81-FDFED6A43D2E}">
   <dimension ref="A1:B9"/>
   <sheetViews>
@@ -1482,7 +1938,7 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="34.85546875" customWidth="1"/>
     <col min="2" max="2" width="29.42578125" customWidth="1"/>
@@ -1540,7 +1996,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{758A37E4-006D-4EC7-A650-6E18768E6BAD}">
   <dimension ref="A1:B6"/>
   <sheetViews>
@@ -1548,7 +2004,7 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="25.42578125" customWidth="1"/>
     <col min="2" max="2" width="29.42578125" customWidth="1"/>
@@ -1597,139 +2053,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{700149C1-66F5-4A24-928F-5BBEDD6006E3}">
-  <dimension ref="A1:B5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="25.5703125" customWidth="1"/>
-    <col min="2" max="2" width="29.42578125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>66</v>
-      </c>
-      <c r="B1" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B2" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>46</v>
-      </c>
-      <c r="B3" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>79</v>
-      </c>
-      <c r="B5" t="s">
-        <v>15</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A7DE5E1-2065-4857-A2CD-738C548B16E2}">
-  <dimension ref="A1:B9"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="35.28515625" customWidth="1"/>
-    <col min="2" max="2" width="72" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B2" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5">
-        <v>500000</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>44</v>
-      </c>
-      <c r="B6">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>8</v>
-      </c>
-      <c r="B8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>10</v>
-      </c>
-      <c r="B9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>